<commit_message>
feat: adding function to handle separately permeability log
</commit_message>
<xml_diff>
--- a/database/test_target.xlsx
+++ b/database/test_target.xlsx
@@ -442,2306 +442,2306 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>962</v>
+        <v>1186</v>
       </c>
       <c r="B2" t="n">
-        <v>2.764561832</v>
+        <v>1.942575764</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1077</v>
+        <v>1868</v>
       </c>
       <c r="B3" t="n">
-        <v>20.60901097</v>
+        <v>15.53263525</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>665</v>
+        <v>264</v>
       </c>
       <c r="B4" t="n">
-        <v>10.40028875</v>
+        <v>5.686513047</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>29</v>
+        <v>559</v>
       </c>
       <c r="B5" t="n">
-        <v>4.929493188</v>
+        <v>10.39197131</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>441</v>
+        <v>363</v>
       </c>
       <c r="B6" t="n">
-        <v>3.609141432</v>
+        <v>6.98542486</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>1190</v>
+        <v>701</v>
       </c>
       <c r="B7" t="n">
-        <v>14.28641271</v>
+        <v>1.377728144</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1162</v>
+        <v>1285</v>
       </c>
       <c r="B8" t="n">
-        <v>13.45629827</v>
+        <v>6.086451365</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>1123</v>
+        <v>1891</v>
       </c>
       <c r="B9" t="n">
-        <v>3.506780718</v>
+        <v>23.36833307</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>704</v>
+        <v>7</v>
       </c>
       <c r="B10" t="n">
-        <v>3.251408955</v>
+        <v>2.866834465</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>922</v>
+        <v>84</v>
       </c>
       <c r="B11" t="n">
-        <v>7.588971112</v>
+        <v>5.704753948</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>540</v>
+        <v>513</v>
       </c>
       <c r="B12" t="n">
-        <v>21.25123704</v>
+        <v>12.36824346</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>454</v>
+        <v>899</v>
       </c>
       <c r="B13" t="n">
-        <v>4.859886452</v>
+        <v>13.04847369</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>248</v>
+        <v>1238</v>
       </c>
       <c r="B14" t="n">
-        <v>11.78700573</v>
+        <v>5.999444069</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>533</v>
+        <v>783</v>
       </c>
       <c r="B15" t="n">
-        <v>11.45365705</v>
+        <v>2.329514472</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>834</v>
+        <v>109</v>
       </c>
       <c r="B16" t="n">
-        <v>10.1797811</v>
+        <v>3.277788138</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>823</v>
+        <v>1859</v>
       </c>
       <c r="B17" t="n">
-        <v>3.583964622</v>
+        <v>12.68853597</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>270</v>
+        <v>4</v>
       </c>
       <c r="B18" t="n">
-        <v>4.501452811</v>
+        <v>2.311590589</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1906</v>
+        <v>585</v>
       </c>
       <c r="B19" t="n">
-        <v>2.525754507</v>
+        <v>2.084117348</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>629</v>
+        <v>1187</v>
       </c>
       <c r="B20" t="n">
-        <v>8.324226356</v>
+        <v>22.69759331</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>450</v>
+        <v>320</v>
       </c>
       <c r="B21" t="n">
-        <v>5.073046797</v>
+        <v>12.09849704</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>446</v>
+        <v>1511</v>
       </c>
       <c r="B22" t="n">
-        <v>1.542989109</v>
+        <v>2.544750724</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>669</v>
+        <v>1502</v>
       </c>
       <c r="B23" t="n">
-        <v>9.890819269</v>
+        <v>18.24622044</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>994</v>
+        <v>373</v>
       </c>
       <c r="B24" t="n">
-        <v>2.206427225</v>
+        <v>9.120455044</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>759</v>
+        <v>889</v>
       </c>
       <c r="B25" t="n">
-        <v>2.039371485</v>
+        <v>1.631425814</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="B26" t="n">
-        <v>1.791903903</v>
+        <v>8.530149106</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>301</v>
+        <v>629</v>
       </c>
       <c r="B27" t="n">
-        <v>3.971635817</v>
+        <v>8.324226356</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>746</v>
+        <v>322</v>
       </c>
       <c r="B28" t="n">
-        <v>4.521125379</v>
+        <v>1.124313668</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1494</v>
+        <v>1165</v>
       </c>
       <c r="B29" t="n">
-        <v>3.191354419</v>
+        <v>18.14542369</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>622</v>
+        <v>236</v>
       </c>
       <c r="B30" t="n">
-        <v>14.5462523</v>
+        <v>2.317056187</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>319</v>
+        <v>1139</v>
       </c>
       <c r="B31" t="n">
-        <v>2.245353382</v>
+        <v>4.883263993</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>948</v>
+        <v>581</v>
       </c>
       <c r="B32" t="n">
-        <v>4.857825405</v>
+        <v>6.836648139</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>114</v>
+        <v>377</v>
       </c>
       <c r="B33" t="n">
-        <v>4.79399121</v>
+        <v>28.30601106</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>902</v>
+        <v>112</v>
       </c>
       <c r="B34" t="n">
-        <v>11.43171708</v>
+        <v>5.468224135</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>1182</v>
+        <v>237</v>
       </c>
       <c r="B35" t="n">
-        <v>0.753988816</v>
+        <v>2.524046975</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>1894</v>
+        <v>746</v>
       </c>
       <c r="B36" t="n">
-        <v>4.70048796</v>
+        <v>4.521125379</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>280</v>
+        <v>1211</v>
       </c>
       <c r="B37" t="n">
-        <v>7.368192608</v>
+        <v>16.82391205</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>1862</v>
+        <v>819</v>
       </c>
       <c r="B38" t="n">
-        <v>6.74986873</v>
+        <v>15.28476912</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>134</v>
+        <v>1564</v>
       </c>
       <c r="B39" t="n">
-        <v>10.37536785</v>
+        <v>4.70907435</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>901</v>
+        <v>786</v>
       </c>
       <c r="B40" t="n">
-        <v>13.58440615</v>
+        <v>1.818488732</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>1285</v>
+        <v>127</v>
       </c>
       <c r="B41" t="n">
-        <v>6.086451365</v>
+        <v>4.788787786</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>213</v>
+        <v>955</v>
       </c>
       <c r="B42" t="n">
-        <v>3.378061513</v>
+        <v>8.836651641</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>1528</v>
+        <v>433</v>
       </c>
       <c r="B43" t="n">
-        <v>4.510608132</v>
+        <v>10.42111694</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>886</v>
+        <v>1497</v>
       </c>
       <c r="B44" t="n">
-        <v>6.18035713</v>
+        <v>3.540119907</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>1516</v>
+        <v>688</v>
       </c>
       <c r="B45" t="n">
-        <v>1.98724572</v>
+        <v>2.536271709</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>1137</v>
+        <v>1007</v>
       </c>
       <c r="B46" t="n">
-        <v>3.938286344</v>
+        <v>0.142013334</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>1216</v>
+        <v>95</v>
       </c>
       <c r="B47" t="n">
-        <v>6.045237669</v>
+        <v>6.954065147</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>1490</v>
+        <v>1551</v>
       </c>
       <c r="B48" t="n">
-        <v>8.910080323000001</v>
+        <v>9.91735877</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>367</v>
+        <v>1199</v>
       </c>
       <c r="B49" t="n">
-        <v>16.7832932</v>
+        <v>4.411343096</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>331</v>
+        <v>176</v>
       </c>
       <c r="B50" t="n">
-        <v>4.556249266</v>
+        <v>5.48061015</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>741</v>
+        <v>406</v>
       </c>
       <c r="B51" t="n">
-        <v>7.04373661</v>
+        <v>3.416166495</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>721</v>
+        <v>810</v>
       </c>
       <c r="B52" t="n">
-        <v>4.634614497</v>
+        <v>16.49421933</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>1907</v>
+        <v>1147</v>
       </c>
       <c r="B53" t="n">
-        <v>3.11258389</v>
+        <v>11.22310967</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>666</v>
+        <v>716</v>
       </c>
       <c r="B54" t="n">
-        <v>7.528913847</v>
+        <v>6.116449971</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>878</v>
+        <v>1145</v>
       </c>
       <c r="B55" t="n">
-        <v>1.711601891</v>
+        <v>1.738204114</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>428</v>
+        <v>1014</v>
       </c>
       <c r="B56" t="n">
-        <v>11.35448293</v>
+        <v>8.225421277000001</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>829</v>
+        <v>1862</v>
       </c>
       <c r="B57" t="n">
-        <v>12.7521176</v>
+        <v>6.74986873</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>810</v>
+        <v>909</v>
       </c>
       <c r="B58" t="n">
-        <v>16.49421933</v>
+        <v>7.618347122</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>460</v>
+        <v>528</v>
       </c>
       <c r="B59" t="n">
-        <v>3.979162541</v>
+        <v>2.210359866</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>1140</v>
+        <v>1305</v>
       </c>
       <c r="B60" t="n">
-        <v>2.242179224</v>
+        <v>14.90202386</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>1303</v>
+        <v>906</v>
       </c>
       <c r="B61" t="n">
-        <v>6.123428801</v>
+        <v>9.478011383</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>109</v>
+        <v>1127</v>
       </c>
       <c r="B62" t="n">
-        <v>3.277788138</v>
+        <v>5.408149469</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>1187</v>
+        <v>386</v>
       </c>
       <c r="B63" t="n">
-        <v>22.69759331</v>
+        <v>7.134468448</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>1873</v>
+        <v>709</v>
       </c>
       <c r="B64" t="n">
-        <v>1.90688641</v>
+        <v>4.360942523</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>1129</v>
+        <v>35</v>
       </c>
       <c r="B65" t="n">
-        <v>7.746258285</v>
+        <v>15.58043619</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>1236</v>
+        <v>484</v>
       </c>
       <c r="B66" t="n">
-        <v>7.262603517</v>
+        <v>10.10143549</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>420</v>
+        <v>911</v>
       </c>
       <c r="B67" t="n">
-        <v>7.643329238</v>
+        <v>4.246184113</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>41</v>
+        <v>1309</v>
       </c>
       <c r="B68" t="n">
-        <v>9.204087916000001</v>
+        <v>4.098475504</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>559</v>
+        <v>602</v>
       </c>
       <c r="B69" t="n">
-        <v>10.39197131</v>
+        <v>2.714115751</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>591</v>
+        <v>827</v>
       </c>
       <c r="B70" t="n">
-        <v>2.15110431</v>
+        <v>3.127403268</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>335</v>
+        <v>760</v>
       </c>
       <c r="B71" t="n">
-        <v>23.2819171</v>
+        <v>2.208487063</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>1511</v>
+        <v>671</v>
       </c>
       <c r="B72" t="n">
-        <v>2.544750724</v>
+        <v>3.608713724</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>1273</v>
+        <v>60</v>
       </c>
       <c r="B73" t="n">
-        <v>8.436190799</v>
+        <v>0.169621487</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>1125</v>
+        <v>257</v>
       </c>
       <c r="B74" t="n">
-        <v>4.452775966</v>
+        <v>6.473995285</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>1899</v>
+        <v>837</v>
       </c>
       <c r="B75" t="n">
-        <v>3.623021496</v>
+        <v>14.85469687</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>93</v>
+        <v>1260</v>
       </c>
       <c r="B76" t="n">
-        <v>3.542055226</v>
+        <v>4.354090239</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>522</v>
+        <v>903</v>
       </c>
       <c r="B77" t="n">
-        <v>3.2624933</v>
+        <v>24.72030173</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>980</v>
+        <v>171</v>
       </c>
       <c r="B78" t="n">
-        <v>1.588763009</v>
+        <v>4.305664972</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>1282</v>
+        <v>765</v>
       </c>
       <c r="B79" t="n">
-        <v>14.44837817</v>
+        <v>5.507124664</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>1060</v>
+        <v>919</v>
       </c>
       <c r="B80" t="n">
-        <v>0.8530261139999999</v>
+        <v>3.515999317</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>1169</v>
+        <v>125</v>
       </c>
       <c r="B81" t="n">
-        <v>11.04032438</v>
+        <v>5.608532732</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>306</v>
+        <v>1873</v>
       </c>
       <c r="B82" t="n">
-        <v>6.619277037</v>
+        <v>1.90688641</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>937</v>
+        <v>110</v>
       </c>
       <c r="B83" t="n">
-        <v>15.16195083</v>
+        <v>4.119795432</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>1206</v>
+        <v>832</v>
       </c>
       <c r="B84" t="n">
-        <v>2.875195382</v>
+        <v>14.64996194</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>729</v>
+        <v>1157</v>
       </c>
       <c r="B85" t="n">
-        <v>17.59077913</v>
+        <v>4.128289298</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>1072</v>
+        <v>1022</v>
       </c>
       <c r="B86" t="n">
-        <v>5.79744199</v>
+        <v>4.4150538</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>1251</v>
+        <v>564</v>
       </c>
       <c r="B87" t="n">
-        <v>18.06646239</v>
+        <v>11.29322897</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>562</v>
+        <v>1298</v>
       </c>
       <c r="B88" t="n">
-        <v>3.007367029</v>
+        <v>2.040259928</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>508</v>
+        <v>379</v>
       </c>
       <c r="B89" t="n">
-        <v>5.917760572</v>
+        <v>9.911599206</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>1138</v>
+        <v>265</v>
       </c>
       <c r="B90" t="n">
-        <v>2.664989196</v>
+        <v>1.682853658</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>219</v>
+        <v>298</v>
       </c>
       <c r="B91" t="n">
-        <v>9.545974185</v>
+        <v>5.868904837</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>302</v>
+        <v>678</v>
       </c>
       <c r="B92" t="n">
-        <v>3.193691363</v>
+        <v>10.19830367</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>1004</v>
+        <v>831</v>
       </c>
       <c r="B93" t="n">
-        <v>0.633755877</v>
+        <v>19.03283303</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>111</v>
+        <v>604</v>
       </c>
       <c r="B94" t="n">
-        <v>8.251959846</v>
+        <v>18.44853818</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>758</v>
+        <v>182</v>
       </c>
       <c r="B95" t="n">
-        <v>1.476919165</v>
+        <v>7.085434186</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>1095</v>
+        <v>590</v>
       </c>
       <c r="B96" t="n">
-        <v>8.580892553</v>
+        <v>7.722099176</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>326</v>
+        <v>1281</v>
       </c>
       <c r="B97" t="n">
-        <v>4.125559426</v>
+        <v>13.51297643</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>487</v>
+        <v>325</v>
       </c>
       <c r="B98" t="n">
-        <v>6.696719792</v>
+        <v>5.728590451</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>97</v>
+        <v>694</v>
       </c>
       <c r="B99" t="n">
-        <v>5.158493248</v>
+        <v>4.000152817</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>440</v>
+        <v>1315</v>
       </c>
       <c r="B100" t="n">
-        <v>5.031238201</v>
+        <v>7.426508774</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>1244</v>
+        <v>1208</v>
       </c>
       <c r="B101" t="n">
-        <v>11.94438288</v>
+        <v>3.919425327</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>1029</v>
+        <v>21</v>
       </c>
       <c r="B102" t="n">
-        <v>1.413595289</v>
+        <v>1.968235026</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>1046</v>
+        <v>1110</v>
       </c>
       <c r="B103" t="n">
-        <v>3.498144204</v>
+        <v>1.420416473</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>871</v>
+        <v>893</v>
       </c>
       <c r="B104" t="n">
-        <v>6.013640915</v>
+        <v>3.451730026</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>1078</v>
+        <v>1135</v>
       </c>
       <c r="B105" t="n">
-        <v>25.15850258</v>
+        <v>7.630535538</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>762</v>
+        <v>1023</v>
       </c>
       <c r="B106" t="n">
-        <v>3.884319996</v>
+        <v>6.306234527</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>771</v>
+        <v>706</v>
       </c>
       <c r="B107" t="n">
-        <v>1.208952334</v>
+        <v>6.298844699</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>419</v>
+        <v>801</v>
       </c>
       <c r="B108" t="n">
-        <v>10.76059384</v>
+        <v>45.27448421</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>893</v>
+        <v>655</v>
       </c>
       <c r="B109" t="n">
-        <v>3.451730026</v>
+        <v>0.780461477</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>180</v>
+        <v>1148</v>
       </c>
       <c r="B110" t="n">
-        <v>4.204086559</v>
+        <v>8.265038085</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>1903</v>
+        <v>393</v>
       </c>
       <c r="B111" t="n">
-        <v>0.866231616</v>
+        <v>4.252570445</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>1286</v>
+        <v>1235</v>
       </c>
       <c r="B112" t="n">
-        <v>26.95200641</v>
+        <v>19.25597407</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>1096</v>
+        <v>1150</v>
       </c>
       <c r="B113" t="n">
-        <v>13.44928477</v>
+        <v>5.244472846</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>1250</v>
+        <v>1202</v>
       </c>
       <c r="B114" t="n">
-        <v>13.24322431</v>
+        <v>6.572059975</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>394</v>
+        <v>222</v>
       </c>
       <c r="B115" t="n">
-        <v>6.635429058</v>
+        <v>14.41066927</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>1912</v>
+        <v>998</v>
       </c>
       <c r="B116" t="n">
-        <v>7.812343926</v>
+        <v>3.516954648</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>1063</v>
+        <v>1053</v>
       </c>
       <c r="B117" t="n">
-        <v>7.347076112</v>
+        <v>0.607173883</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>1496</v>
+        <v>1241</v>
       </c>
       <c r="B118" t="n">
-        <v>1.64945067</v>
+        <v>4.317230611</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>982</v>
+        <v>58</v>
       </c>
       <c r="B119" t="n">
-        <v>3.451326361</v>
+        <v>3.704182734</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>1014</v>
+        <v>1080</v>
       </c>
       <c r="B120" t="n">
-        <v>8.225421277000001</v>
+        <v>10.44133384</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>147</v>
+        <v>504</v>
       </c>
       <c r="B121" t="n">
-        <v>27.75018732</v>
+        <v>14.25321389</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>1157</v>
+        <v>984</v>
       </c>
       <c r="B122" t="n">
-        <v>4.128289298</v>
+        <v>7.524731836</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>542</v>
+        <v>551</v>
       </c>
       <c r="B123" t="n">
-        <v>28.00292599</v>
+        <v>7.936765267</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>577</v>
+        <v>0</v>
       </c>
       <c r="B124" t="n">
-        <v>12.61850799</v>
+        <v>8.422064636</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>710</v>
+        <v>549</v>
       </c>
       <c r="B125" t="n">
-        <v>6.376827688</v>
+        <v>6.585174826</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>751</v>
+        <v>796</v>
       </c>
       <c r="B126" t="n">
-        <v>2.879892495</v>
+        <v>16.78183408</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>961</v>
+        <v>331</v>
       </c>
       <c r="B127" t="n">
-        <v>9.541877105999999</v>
+        <v>4.556249266</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>1527</v>
+        <v>1170</v>
       </c>
       <c r="B128" t="n">
-        <v>0.717175871</v>
+        <v>11.35464727</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>361</v>
+        <v>56</v>
       </c>
       <c r="B129" t="n">
-        <v>6.43839193</v>
+        <v>9.299167942</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>456</v>
+        <v>1217</v>
       </c>
       <c r="B130" t="n">
-        <v>10.15147821</v>
+        <v>8.551846208000001</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>18</v>
+        <v>1265</v>
       </c>
       <c r="B131" t="n">
-        <v>0.830471344</v>
+        <v>14.84067376</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>863</v>
+        <v>92</v>
       </c>
       <c r="B132" t="n">
-        <v>6.312758056</v>
+        <v>9.361645508000001</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>900</v>
+        <v>1206</v>
       </c>
       <c r="B133" t="n">
-        <v>7.328221334</v>
+        <v>2.875195382</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>1313</v>
+        <v>663</v>
       </c>
       <c r="B134" t="n">
-        <v>7.866193029</v>
+        <v>13.81309878</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>590</v>
+        <v>649</v>
       </c>
       <c r="B135" t="n">
-        <v>7.722099176</v>
+        <v>3.592411721</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="B136" t="n">
-        <v>18.42587021</v>
+        <v>5.767574894</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>1260</v>
+        <v>863</v>
       </c>
       <c r="B137" t="n">
-        <v>4.354090239</v>
+        <v>6.312758056</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>686</v>
+        <v>1515</v>
       </c>
       <c r="B138" t="n">
-        <v>3.084074667</v>
+        <v>1.241706504</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>816</v>
+        <v>1294</v>
       </c>
       <c r="B139" t="n">
-        <v>7.949328139</v>
+        <v>4.715966204</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>703</v>
+        <v>548</v>
       </c>
       <c r="B140" t="n">
-        <v>2.4483074</v>
+        <v>5.893807862</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>1550</v>
+        <v>422</v>
       </c>
       <c r="B141" t="n">
-        <v>6.577247291</v>
+        <v>19.60390138</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>808</v>
+        <v>1195</v>
       </c>
       <c r="B142" t="n">
-        <v>10.29414117</v>
+        <v>1.791163332</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>505</v>
+        <v>292</v>
       </c>
       <c r="B143" t="n">
-        <v>20.15083283</v>
+        <v>3.516943532</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>812</v>
+        <v>1508</v>
       </c>
       <c r="B144" t="n">
-        <v>11.88318456</v>
+        <v>5.593399546</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>466</v>
+        <v>199</v>
       </c>
       <c r="B145" t="n">
-        <v>9.031869403</v>
+        <v>6.176411989</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>314</v>
+        <v>1874</v>
       </c>
       <c r="B146" t="n">
-        <v>3.325326956</v>
+        <v>2.254280661</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>75</v>
+        <v>485</v>
       </c>
       <c r="B147" t="n">
-        <v>2.69255836</v>
+        <v>5.355498109</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>1257</v>
+        <v>1027</v>
       </c>
       <c r="B148" t="n">
-        <v>10.93955763</v>
+        <v>3.48814515</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>66</v>
+        <v>1310</v>
       </c>
       <c r="B149" t="n">
-        <v>5.714807752</v>
+        <v>8.575790831999999</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>1500</v>
+        <v>146</v>
       </c>
       <c r="B150" t="n">
-        <v>6.512056904</v>
+        <v>56.08509159</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>604</v>
+        <v>1312</v>
       </c>
       <c r="B151" t="n">
-        <v>18.44853818</v>
+        <v>15.50679647</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>188</v>
+        <v>357</v>
       </c>
       <c r="B152" t="n">
-        <v>7.751241315</v>
+        <v>5.718274897</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>644</v>
+        <v>1233</v>
       </c>
       <c r="B153" t="n">
-        <v>9.965740084</v>
+        <v>8.50162531</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>1105</v>
+        <v>1558</v>
       </c>
       <c r="B154" t="n">
-        <v>34.67373448</v>
+        <v>6.923547824</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>785</v>
+        <v>163</v>
       </c>
       <c r="B155" t="n">
-        <v>3.259647577</v>
+        <v>5.747322623</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>585</v>
+        <v>994</v>
       </c>
       <c r="B156" t="n">
-        <v>2.084117348</v>
+        <v>2.206427225</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>1213</v>
+        <v>1074</v>
       </c>
       <c r="B157" t="n">
-        <v>7.907118123</v>
+        <v>10.59243092</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>464</v>
+        <v>1121</v>
       </c>
       <c r="B158" t="n">
-        <v>4.921387479</v>
+        <v>7.753343084</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>935</v>
+        <v>961</v>
       </c>
       <c r="B159" t="n">
-        <v>10.77448021</v>
+        <v>9.541877105999999</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>694</v>
+        <v>1514</v>
       </c>
       <c r="B160" t="n">
-        <v>4.000152817</v>
+        <v>2.923991011</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>468</v>
+        <v>995</v>
       </c>
       <c r="B161" t="n">
-        <v>9.204340435000001</v>
+        <v>3.933971262</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>1551</v>
+        <v>244</v>
       </c>
       <c r="B162" t="n">
-        <v>9.91735877</v>
+        <v>8.333593296</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>667</v>
+        <v>1221</v>
       </c>
       <c r="B163" t="n">
-        <v>5.130884132</v>
+        <v>18.16059629</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>1876</v>
+        <v>651</v>
       </c>
       <c r="B164" t="n">
-        <v>4.341231829</v>
+        <v>1.542364563</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>13</v>
+        <v>1087</v>
       </c>
       <c r="B165" t="n">
-        <v>9.378950159</v>
+        <v>19.30242725</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>1243</v>
+        <v>81</v>
       </c>
       <c r="B166" t="n">
-        <v>9.546853707</v>
+        <v>7.002961284</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>1278</v>
+        <v>935</v>
       </c>
       <c r="B167" t="n">
-        <v>5.996995082</v>
+        <v>10.77448021</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>747</v>
+        <v>517</v>
       </c>
       <c r="B168" t="n">
-        <v>3.500439066</v>
+        <v>15.68333812</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B169" t="n">
-        <v>1.371743446</v>
+        <v>6.213209469</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
-        <v>530</v>
+        <v>937</v>
       </c>
       <c r="B170" t="n">
-        <v>6.573594731</v>
+        <v>15.16195083</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>998</v>
+        <v>722</v>
       </c>
       <c r="B171" t="n">
-        <v>3.516954648</v>
+        <v>5.255192675</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>712</v>
+        <v>664</v>
       </c>
       <c r="B172" t="n">
-        <v>3.048842812</v>
+        <v>22.2533743</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>913</v>
+        <v>965</v>
       </c>
       <c r="B173" t="n">
-        <v>4.217561936</v>
+        <v>8.051653369</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>292</v>
+        <v>202</v>
       </c>
       <c r="B174" t="n">
-        <v>3.516943532</v>
+        <v>15.35336526</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
-        <v>1297</v>
+        <v>418</v>
       </c>
       <c r="B175" t="n">
-        <v>4.719863568</v>
+        <v>9.871273872</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>333</v>
+        <v>3</v>
       </c>
       <c r="B176" t="n">
-        <v>4.485715333</v>
+        <v>7.893081934</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B177" t="n">
-        <v>2.311590589</v>
+        <v>6.628267212</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
-        <v>387</v>
+        <v>1154</v>
       </c>
       <c r="B178" t="n">
-        <v>23.39032556</v>
+        <v>3.00723487</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>150</v>
+        <v>305</v>
       </c>
       <c r="B179" t="n">
-        <v>6.406698007</v>
+        <v>11.34589481</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>1089</v>
+        <v>764</v>
       </c>
       <c r="B180" t="n">
-        <v>6.737976625</v>
+        <v>9.197091886999999</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>187</v>
+        <v>516</v>
       </c>
       <c r="B181" t="n">
-        <v>6.249381229</v>
+        <v>11.96201208</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>1080</v>
+        <v>892</v>
       </c>
       <c r="B182" t="n">
-        <v>10.44133384</v>
+        <v>3.379699033</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>740</v>
+        <v>1856</v>
       </c>
       <c r="B183" t="n">
-        <v>3.745027624</v>
+        <v>6.783337842</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
-        <v>264</v>
+        <v>784</v>
       </c>
       <c r="B184" t="n">
-        <v>5.686513047</v>
+        <v>3.154616194</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>774</v>
+        <v>1075</v>
       </c>
       <c r="B185" t="n">
-        <v>1.396188362</v>
+        <v>11.22339524</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
-        <v>583</v>
+        <v>834</v>
       </c>
       <c r="B186" t="n">
-        <v>4.187765314</v>
+        <v>10.1797811</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
-        <v>676</v>
+        <v>1864</v>
       </c>
       <c r="B187" t="n">
-        <v>7.344485921</v>
+        <v>6.938495397</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>819</v>
+        <v>1545</v>
       </c>
       <c r="B188" t="n">
-        <v>15.28476912</v>
+        <v>5.094255712</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>6</v>
+        <v>468</v>
       </c>
       <c r="B189" t="n">
-        <v>6.291019906</v>
+        <v>9.204340435000001</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>527</v>
+        <v>1236</v>
       </c>
       <c r="B190" t="n">
-        <v>18.66711301</v>
+        <v>7.262603517</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>1890</v>
+        <v>212</v>
       </c>
       <c r="B191" t="n">
-        <v>20.03406004</v>
+        <v>4.149723633</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
-        <v>43</v>
+        <v>1904</v>
       </c>
       <c r="B192" t="n">
-        <v>12.24741717</v>
+        <v>7.794791907</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>1173</v>
+        <v>1167</v>
       </c>
       <c r="B193" t="n">
-        <v>5.787170496</v>
+        <v>21.24727776</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>722</v>
+        <v>1094</v>
       </c>
       <c r="B194" t="n">
-        <v>5.255192675</v>
+        <v>9.457559951</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
-        <v>1126</v>
+        <v>482</v>
       </c>
       <c r="B195" t="n">
-        <v>5.380324494</v>
+        <v>66.20402687000001</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
-        <v>679</v>
+        <v>554</v>
       </c>
       <c r="B196" t="n">
-        <v>7.821914928</v>
+        <v>4.400345325</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
-        <v>728</v>
+        <v>1550</v>
       </c>
       <c r="B197" t="n">
-        <v>13.9293069</v>
+        <v>6.577247291</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
-        <v>626</v>
+        <v>344</v>
       </c>
       <c r="B198" t="n">
-        <v>29.89989391</v>
+        <v>16.97827624</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
-        <v>1031</v>
+        <v>1905</v>
       </c>
       <c r="B199" t="n">
-        <v>5.855834883</v>
+        <v>4.246744498</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
-        <v>95</v>
+        <v>508</v>
       </c>
       <c r="B200" t="n">
-        <v>6.954065147</v>
+        <v>5.917760572</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
-        <v>573</v>
+        <v>874</v>
       </c>
       <c r="B201" t="n">
-        <v>6.425386489</v>
+        <v>3.398649395</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>291</v>
+        <v>620</v>
       </c>
       <c r="B202" t="n">
-        <v>4.585579859</v>
+        <v>12.67827277</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>1028</v>
+        <v>1561</v>
       </c>
       <c r="B203" t="n">
-        <v>0.636684326</v>
+        <v>7.446748488</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>1143</v>
+        <v>239</v>
       </c>
       <c r="B204" t="n">
-        <v>2.185066883</v>
+        <v>2.299742102</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>529</v>
+        <v>1123</v>
       </c>
       <c r="B205" t="n">
-        <v>1.983768609</v>
+        <v>3.506780718</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>1891</v>
+        <v>63</v>
       </c>
       <c r="B206" t="n">
-        <v>23.36833307</v>
+        <v>12.36270136</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>38</v>
+        <v>929</v>
       </c>
       <c r="B207" t="n">
-        <v>19.1159843</v>
+        <v>2.348164872</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>553</v>
+        <v>1112</v>
       </c>
       <c r="B208" t="n">
-        <v>8.848099134</v>
+        <v>3.583791072</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>1155</v>
+        <v>141</v>
       </c>
       <c r="B209" t="n">
-        <v>0.885496578</v>
+        <v>4.486268468</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>1916</v>
+        <v>210</v>
       </c>
       <c r="B210" t="n">
-        <v>10.34570918</v>
+        <v>2.370623479</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>633</v>
+        <v>269</v>
       </c>
       <c r="B211" t="n">
-        <v>2.555399578</v>
+        <v>11.00657433</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="B212" t="n">
-        <v>4.963988366</v>
+        <v>6.651263691</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>214</v>
+        <v>1038</v>
       </c>
       <c r="B213" t="n">
-        <v>0.965728467</v>
+        <v>4.282608197</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>1086</v>
+        <v>1026</v>
       </c>
       <c r="B214" t="n">
-        <v>9.193045565</v>
+        <v>4.823260956</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>375</v>
+        <v>922</v>
       </c>
       <c r="B215" t="n">
-        <v>15.5677777</v>
+        <v>7.588971112</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>146</v>
+        <v>436</v>
       </c>
       <c r="B216" t="n">
-        <v>56.08509159</v>
+        <v>15.75945716</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>1176</v>
+        <v>1081</v>
       </c>
       <c r="B217" t="n">
-        <v>4.547074341</v>
+        <v>3.216697166</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>1242</v>
+        <v>397</v>
       </c>
       <c r="B218" t="n">
-        <v>9.316208521</v>
+        <v>5.860503031</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B219" t="n">
-        <v>17.85570215</v>
+        <v>6.363634576</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>1115</v>
+        <v>875</v>
       </c>
       <c r="B220" t="n">
-        <v>10.25195305</v>
+        <v>3.191287868</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>352</v>
+        <v>243</v>
       </c>
       <c r="B221" t="n">
-        <v>5.846572498</v>
+        <v>7.37537074</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>1893</v>
+        <v>1103</v>
       </c>
       <c r="B222" t="n">
-        <v>5.762078035</v>
+        <v>4.080288815</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>867</v>
+        <v>1109</v>
       </c>
       <c r="B223" t="n">
-        <v>4.11229907</v>
+        <v>5.265473643</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>1052</v>
+        <v>1230</v>
       </c>
       <c r="B224" t="n">
-        <v>0.374115401</v>
+        <v>13.43379293</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>1858</v>
+        <v>703</v>
       </c>
       <c r="B225" t="n">
-        <v>10.26421971</v>
+        <v>2.4483074</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>798</v>
+        <v>178</v>
       </c>
       <c r="B226" t="n">
-        <v>13.11127266</v>
+        <v>8.775490261</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>1221</v>
+        <v>415</v>
       </c>
       <c r="B227" t="n">
-        <v>18.16059629</v>
+        <v>3.723703389</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>1012</v>
+        <v>1205</v>
       </c>
       <c r="B228" t="n">
-        <v>4.834334103</v>
+        <v>4.942861368</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>927</v>
+        <v>183</v>
       </c>
       <c r="B229" t="n">
-        <v>15.52151524</v>
+        <v>7.57637515</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>385</v>
+        <v>1512</v>
       </c>
       <c r="B230" t="n">
-        <v>11.95362461</v>
+        <v>3.225325189</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>1136</v>
+        <v>518</v>
       </c>
       <c r="B231" t="n">
-        <v>5.927035504</v>
+        <v>10.97908896</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>1265</v>
+        <v>589</v>
       </c>
       <c r="B232" t="n">
-        <v>14.84067376</v>
+        <v>11.38852803</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>1131</v>
+        <v>524</v>
       </c>
       <c r="B233" t="n">
-        <v>12.68248508</v>
+        <v>1.552124508</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>1082</v>
+        <v>1024</v>
       </c>
       <c r="B234" t="n">
-        <v>2.325112666</v>
+        <v>10.03780942</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>240</v>
+        <v>1253</v>
       </c>
       <c r="B235" t="n">
-        <v>3.471593872</v>
+        <v>7.018089904</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>990</v>
+        <v>324</v>
       </c>
       <c r="B236" t="n">
-        <v>4.714887296</v>
+        <v>5.072832642</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>983</v>
+        <v>630</v>
       </c>
       <c r="B237" t="n">
-        <v>6.168505989</v>
+        <v>10.5803892</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>421</v>
+        <v>1256</v>
       </c>
       <c r="B238" t="n">
-        <v>13.81816867</v>
+        <v>3.799273955</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>1048</v>
+        <v>529</v>
       </c>
       <c r="B239" t="n">
-        <v>0.99917488</v>
+        <v>1.983768609</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>365</v>
+        <v>313</v>
       </c>
       <c r="B240" t="n">
-        <v>7.548358182</v>
+        <v>6.623461771</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>617</v>
+        <v>1131</v>
       </c>
       <c r="B241" t="n">
-        <v>7.138813282</v>
+        <v>12.68248508</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>1495</v>
+        <v>1270</v>
       </c>
       <c r="B242" t="n">
-        <v>6.670454147</v>
+        <v>23.77493671</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>186</v>
+        <v>1047</v>
       </c>
       <c r="B243" t="n">
-        <v>6.054159148</v>
+        <v>0.921319068</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>229</v>
+        <v>536</v>
       </c>
       <c r="B244" t="n">
-        <v>4.386538034</v>
+        <v>9.919362102999999</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>1559</v>
+        <v>1043</v>
       </c>
       <c r="B245" t="n">
-        <v>7.190723156</v>
+        <v>7.001765162</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>689</v>
+        <v>1212</v>
       </c>
       <c r="B246" t="n">
-        <v>2.191520665</v>
+        <v>6.92781315</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>411</v>
+        <v>342</v>
       </c>
       <c r="B247" t="n">
-        <v>11.37703659</v>
+        <v>21.20265521</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>1489</v>
+        <v>266</v>
       </c>
       <c r="B248" t="n">
-        <v>11.37181113</v>
+        <v>0.116309274</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>1026</v>
+        <v>382</v>
       </c>
       <c r="B249" t="n">
-        <v>4.823260956</v>
+        <v>11.84391172</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>925</v>
+        <v>55</v>
       </c>
       <c r="B250" t="n">
-        <v>6.338387506</v>
+        <v>6.380772234</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>516</v>
+        <v>772</v>
       </c>
       <c r="B251" t="n">
-        <v>11.96201208</v>
+        <v>1.236380128</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>632</v>
+        <v>653</v>
       </c>
       <c r="B252" t="n">
-        <v>3.366110403</v>
+        <v>4.149255304</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>1507</v>
+        <v>78</v>
       </c>
       <c r="B253" t="n">
-        <v>3.886821308</v>
+        <v>3.869189366</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>342</v>
+        <v>303</v>
       </c>
       <c r="B254" t="n">
-        <v>21.20265521</v>
+        <v>6.137564282</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>1510</v>
+        <v>1901</v>
       </c>
       <c r="B255" t="n">
-        <v>5.564377222</v>
+        <v>2.443573166</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
-        <v>1079</v>
+        <v>734</v>
       </c>
       <c r="B256" t="n">
-        <v>17.51599246</v>
+        <v>20.83637147</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
-        <v>266</v>
+        <v>1895</v>
       </c>
       <c r="B257" t="n">
-        <v>0.116309274</v>
+        <v>2.214552252</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>868</v>
+        <v>741</v>
       </c>
       <c r="B258" t="n">
-        <v>5.484665541</v>
+        <v>7.04373661</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>1073</v>
+        <v>845</v>
       </c>
       <c r="B259" t="n">
-        <v>6.872368933</v>
+        <v>3.77125118</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>1885</v>
+        <v>618</v>
       </c>
       <c r="B260" t="n">
-        <v>7.776038408</v>
+        <v>3.946696433</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>251</v>
+        <v>149</v>
       </c>
       <c r="B261" t="n">
-        <v>10.25520642</v>
+        <v>3.286599325</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>668</v>
+        <v>767</v>
       </c>
       <c r="B262" t="n">
-        <v>5.33836034</v>
+        <v>2.031511318</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>821</v>
+        <v>594</v>
       </c>
       <c r="B263" t="n">
-        <v>17.46716632</v>
+        <v>10.32004246</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>1066</v>
+        <v>843</v>
       </c>
       <c r="B264" t="n">
-        <v>8.584570329</v>
+        <v>4.719541631</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>1065</v>
+        <v>1870</v>
       </c>
       <c r="B265" t="n">
-        <v>3.787598225</v>
+        <v>9.076710616</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>955</v>
+        <v>1119</v>
       </c>
       <c r="B266" t="n">
-        <v>8.836651641</v>
+        <v>8.436594728999999</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>931</v>
+        <v>284</v>
       </c>
       <c r="B267" t="n">
-        <v>6.510452288</v>
+        <v>12.37242061</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>484</v>
+        <v>755</v>
       </c>
       <c r="B268" t="n">
-        <v>10.10143549</v>
+        <v>16.58343578</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>544</v>
+        <v>369</v>
       </c>
       <c r="B269" t="n">
-        <v>10.29197805</v>
+        <v>3.215905681</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>733</v>
+        <v>22</v>
       </c>
       <c r="B270" t="n">
-        <v>14.47731286</v>
+        <v>1.689171042</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>930</v>
+        <v>915</v>
       </c>
       <c r="B271" t="n">
-        <v>13.5920766</v>
+        <v>6.713584882</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>1548</v>
+        <v>147</v>
       </c>
       <c r="B272" t="n">
-        <v>6.706362305</v>
+        <v>27.75018732</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>1263</v>
+        <v>1886</v>
       </c>
       <c r="B273" t="n">
-        <v>5.757482156</v>
+        <v>5.49698452</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
-        <v>1311</v>
+        <v>882</v>
       </c>
       <c r="B274" t="n">
-        <v>8.258760962</v>
+        <v>0.85139524</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
-        <v>21</v>
+        <v>499</v>
       </c>
       <c r="B275" t="n">
-        <v>1.968235026</v>
+        <v>1.78924921</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
-        <v>552</v>
+        <v>753</v>
       </c>
       <c r="B276" t="n">
-        <v>25.53613408</v>
+        <v>13.20509137</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>1205</v>
+        <v>152</v>
       </c>
       <c r="B277" t="n">
-        <v>4.942861368</v>
+        <v>3.448185178</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
-        <v>344</v>
+        <v>375</v>
       </c>
       <c r="B278" t="n">
-        <v>16.97827624</v>
+        <v>15.5677777</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
-        <v>1120</v>
+        <v>546</v>
       </c>
       <c r="B279" t="n">
-        <v>1.576190242</v>
+        <v>4.169698838</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="B280" t="n">
-        <v>13.81309878</v>
+        <v>8.202778093999999</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
-        <v>99</v>
+        <v>829</v>
       </c>
       <c r="B281" t="n">
-        <v>15.35063654</v>
+        <v>12.7521176</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>274</v>
+        <v>437</v>
       </c>
       <c r="B282" t="n">
-        <v>3.740744636</v>
+        <v>22.28714236</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>839</v>
+        <v>522</v>
       </c>
       <c r="B283" t="n">
-        <v>8.799365691</v>
+        <v>3.2624933</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
-        <v>157</v>
+        <v>885</v>
       </c>
       <c r="B284" t="n">
-        <v>25.40588789</v>
+        <v>8.132012255999999</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
-        <v>204</v>
+        <v>73</v>
       </c>
       <c r="B285" t="n">
-        <v>8.806284267000001</v>
+        <v>1.045292237</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
-        <v>407</v>
+        <v>33</v>
       </c>
       <c r="B286" t="n">
-        <v>10.74531421</v>
+        <v>12.57367205</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
-        <v>1011</v>
+        <v>941</v>
       </c>
       <c r="B287" t="n">
-        <v>11.41160557</v>
+        <v>6.918548492</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
-        <v>1532</v>
+        <v>987</v>
       </c>
       <c r="B288" t="n">
-        <v>6.045093362</v>
+        <v>16.65102368</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
-        <v>1057</v>
+        <v>1898</v>
       </c>
       <c r="B289" t="n">
-        <v>4.270894301</v>
+        <v>2.43695945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: adding modelling class to handle models
</commit_message>
<xml_diff>
--- a/database/test_target.xlsx
+++ b/database/test_target.xlsx
@@ -442,2306 +442,2306 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1186</v>
+        <v>57</v>
       </c>
       <c r="B2" t="n">
-        <v>1.942575764</v>
+        <v>3.714938801</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1868</v>
+        <v>592</v>
       </c>
       <c r="B3" t="n">
-        <v>15.53263525</v>
+        <v>5.700375292</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>264</v>
+        <v>332</v>
       </c>
       <c r="B4" t="n">
-        <v>5.686513047</v>
+        <v>6.119201734</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>559</v>
+        <v>1500</v>
       </c>
       <c r="B5" t="n">
-        <v>10.39197131</v>
+        <v>6.512056904</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>363</v>
+        <v>555</v>
       </c>
       <c r="B6" t="n">
-        <v>6.98542486</v>
+        <v>15.70178671</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>701</v>
+        <v>79</v>
       </c>
       <c r="B7" t="n">
-        <v>1.377728144</v>
+        <v>6.213209469</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>1285</v>
+        <v>655</v>
       </c>
       <c r="B8" t="n">
-        <v>6.086451365</v>
+        <v>0.780461477</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>1891</v>
+        <v>1141</v>
       </c>
       <c r="B9" t="n">
-        <v>23.36833307</v>
+        <v>3.128622525</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>7</v>
+        <v>790</v>
       </c>
       <c r="B10" t="n">
-        <v>2.866834465</v>
+        <v>7.663719303</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>84</v>
+        <v>1058</v>
       </c>
       <c r="B11" t="n">
-        <v>5.704753948</v>
+        <v>4.367109956</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>513</v>
+        <v>76</v>
       </c>
       <c r="B12" t="n">
-        <v>12.36824346</v>
+        <v>3.079469421</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>899</v>
+        <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>13.04847369</v>
+        <v>8.594029848</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1238</v>
+        <v>403</v>
       </c>
       <c r="B14" t="n">
-        <v>5.999444069</v>
+        <v>25.12113925</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>783</v>
+        <v>1523</v>
       </c>
       <c r="B15" t="n">
-        <v>2.329514472</v>
+        <v>1.950020742</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>109</v>
+        <v>1105</v>
       </c>
       <c r="B16" t="n">
-        <v>3.277788138</v>
+        <v>34.67373448</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>1859</v>
+        <v>476</v>
       </c>
       <c r="B17" t="n">
-        <v>12.68853597</v>
+        <v>7.327226503</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>4</v>
+        <v>903</v>
       </c>
       <c r="B18" t="n">
-        <v>2.311590589</v>
+        <v>24.72030173</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>585</v>
+        <v>869</v>
       </c>
       <c r="B19" t="n">
-        <v>2.084117348</v>
+        <v>9.738307656</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>1187</v>
+        <v>645</v>
       </c>
       <c r="B20" t="n">
-        <v>22.69759331</v>
+        <v>9.707002576000001</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>320</v>
+        <v>906</v>
       </c>
       <c r="B21" t="n">
-        <v>12.09849704</v>
+        <v>9.478011383</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1511</v>
+        <v>5</v>
       </c>
       <c r="B22" t="n">
-        <v>2.544750724</v>
+        <v>3.988171652</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>1502</v>
+        <v>1130</v>
       </c>
       <c r="B23" t="n">
-        <v>18.24622044</v>
+        <v>11.57489251</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>373</v>
+        <v>777</v>
       </c>
       <c r="B24" t="n">
-        <v>9.120455044</v>
+        <v>4.556289426</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>889</v>
+        <v>844</v>
       </c>
       <c r="B25" t="n">
-        <v>1.631425814</v>
+        <v>7.874104063</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>96</v>
+        <v>972</v>
       </c>
       <c r="B26" t="n">
-        <v>8.530149106</v>
+        <v>1.578940541</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>629</v>
+        <v>965</v>
       </c>
       <c r="B27" t="n">
-        <v>8.324226356</v>
+        <v>8.051653369</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>322</v>
+        <v>1266</v>
       </c>
       <c r="B28" t="n">
-        <v>1.124313668</v>
+        <v>7.556753699</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1165</v>
+        <v>1300</v>
       </c>
       <c r="B29" t="n">
-        <v>18.14542369</v>
+        <v>4.832673313</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>236</v>
+        <v>85</v>
       </c>
       <c r="B30" t="n">
-        <v>2.317056187</v>
+        <v>11.6596888</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>1139</v>
+        <v>684</v>
       </c>
       <c r="B31" t="n">
-        <v>4.883263993</v>
+        <v>5.847297682</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>581</v>
+        <v>152</v>
       </c>
       <c r="B32" t="n">
-        <v>6.836648139</v>
+        <v>3.448185178</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>377</v>
+        <v>1009</v>
       </c>
       <c r="B33" t="n">
-        <v>28.30601106</v>
+        <v>6.263496579</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>112</v>
+        <v>1182</v>
       </c>
       <c r="B34" t="n">
-        <v>5.468224135</v>
+        <v>0.753988816</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>237</v>
+        <v>546</v>
       </c>
       <c r="B35" t="n">
-        <v>2.524046975</v>
+        <v>4.169698838</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>746</v>
+        <v>1561</v>
       </c>
       <c r="B36" t="n">
-        <v>4.521125379</v>
+        <v>7.446748488</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>1211</v>
+        <v>89</v>
       </c>
       <c r="B37" t="n">
-        <v>16.82391205</v>
+        <v>5.30582184</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>819</v>
+        <v>562</v>
       </c>
       <c r="B38" t="n">
-        <v>15.28476912</v>
+        <v>3.007367029</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>1564</v>
+        <v>153</v>
       </c>
       <c r="B39" t="n">
-        <v>4.70907435</v>
+        <v>1.551707049</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>786</v>
+        <v>683</v>
       </c>
       <c r="B40" t="n">
-        <v>1.818488732</v>
+        <v>5.508617681</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>127</v>
+        <v>522</v>
       </c>
       <c r="B41" t="n">
-        <v>4.788787786</v>
+        <v>3.2624933</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>955</v>
+        <v>250</v>
       </c>
       <c r="B42" t="n">
-        <v>8.836651641</v>
+        <v>6.562449049</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>433</v>
+        <v>144</v>
       </c>
       <c r="B43" t="n">
-        <v>10.42111694</v>
+        <v>6.034439596</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>1497</v>
+        <v>151</v>
       </c>
       <c r="B44" t="n">
-        <v>3.540119907</v>
+        <v>4.963988366</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>688</v>
+        <v>197</v>
       </c>
       <c r="B45" t="n">
-        <v>2.536271709</v>
+        <v>20.47621221</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>1007</v>
+        <v>366</v>
       </c>
       <c r="B46" t="n">
-        <v>0.142013334</v>
+        <v>15.03867485</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>95</v>
+        <v>259</v>
       </c>
       <c r="B47" t="n">
-        <v>6.954065147</v>
+        <v>3.539583828</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>1551</v>
+        <v>104</v>
       </c>
       <c r="B48" t="n">
-        <v>9.91735877</v>
+        <v>1.167620554</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>1199</v>
+        <v>1092</v>
       </c>
       <c r="B49" t="n">
-        <v>4.411343096</v>
+        <v>13.42538649</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>176</v>
+        <v>1212</v>
       </c>
       <c r="B50" t="n">
-        <v>5.48061015</v>
+        <v>6.92781315</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>406</v>
+        <v>544</v>
       </c>
       <c r="B51" t="n">
-        <v>3.416166495</v>
+        <v>10.29197805</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>810</v>
+        <v>944</v>
       </c>
       <c r="B52" t="n">
-        <v>16.49421933</v>
+        <v>25.85730478</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>1147</v>
+        <v>339</v>
       </c>
       <c r="B53" t="n">
-        <v>11.22310967</v>
+        <v>0.810924655</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>716</v>
+        <v>176</v>
       </c>
       <c r="B54" t="n">
-        <v>6.116449971</v>
+        <v>5.48061015</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>1145</v>
+        <v>1269</v>
       </c>
       <c r="B55" t="n">
-        <v>1.738204114</v>
+        <v>7.536202212</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>1014</v>
+        <v>542</v>
       </c>
       <c r="B56" t="n">
-        <v>8.225421277000001</v>
+        <v>28.00292599</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>1862</v>
+        <v>322</v>
       </c>
       <c r="B57" t="n">
-        <v>6.74986873</v>
+        <v>1.124313668</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>909</v>
+        <v>961</v>
       </c>
       <c r="B58" t="n">
-        <v>7.618347122</v>
+        <v>9.541877105999999</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>528</v>
+        <v>75</v>
       </c>
       <c r="B59" t="n">
-        <v>2.210359866</v>
+        <v>2.69255836</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>1305</v>
+        <v>447</v>
       </c>
       <c r="B60" t="n">
-        <v>14.90202386</v>
+        <v>3.310632596</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>906</v>
+        <v>440</v>
       </c>
       <c r="B61" t="n">
-        <v>9.478011383</v>
+        <v>5.031238201</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>1127</v>
+        <v>413</v>
       </c>
       <c r="B62" t="n">
-        <v>5.408149469</v>
+        <v>2.130954349</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>386</v>
+        <v>755</v>
       </c>
       <c r="B63" t="n">
-        <v>7.134468448</v>
+        <v>16.58343578</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>709</v>
+        <v>1254</v>
       </c>
       <c r="B64" t="n">
-        <v>4.360942523</v>
+        <v>5.599847898</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>35</v>
+        <v>957</v>
       </c>
       <c r="B65" t="n">
-        <v>15.58043619</v>
+        <v>5.070651108</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>484</v>
+        <v>536</v>
       </c>
       <c r="B66" t="n">
-        <v>10.10143549</v>
+        <v>9.919362102999999</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>911</v>
+        <v>1072</v>
       </c>
       <c r="B67" t="n">
-        <v>4.246184113</v>
+        <v>5.79744199</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>1309</v>
+        <v>145</v>
       </c>
       <c r="B68" t="n">
-        <v>4.098475504</v>
+        <v>20.27307482</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>602</v>
+        <v>1233</v>
       </c>
       <c r="B69" t="n">
-        <v>2.714115751</v>
+        <v>8.50162531</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>827</v>
+        <v>743</v>
       </c>
       <c r="B70" t="n">
-        <v>3.127403268</v>
+        <v>6.341233607</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>760</v>
+        <v>405</v>
       </c>
       <c r="B71" t="n">
-        <v>2.208487063</v>
+        <v>8.044392311999999</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>671</v>
+        <v>1238</v>
       </c>
       <c r="B72" t="n">
-        <v>3.608713724</v>
+        <v>5.999444069</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>60</v>
+        <v>186</v>
       </c>
       <c r="B73" t="n">
-        <v>0.169621487</v>
+        <v>6.054159148</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>257</v>
+        <v>341</v>
       </c>
       <c r="B74" t="n">
-        <v>6.473995285</v>
+        <v>6.428348155</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>837</v>
+        <v>1522</v>
       </c>
       <c r="B75" t="n">
-        <v>14.85469687</v>
+        <v>5.378715114</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>1260</v>
+        <v>313</v>
       </c>
       <c r="B76" t="n">
-        <v>4.354090239</v>
+        <v>6.623461771</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>903</v>
+        <v>586</v>
       </c>
       <c r="B77" t="n">
-        <v>24.72030173</v>
+        <v>7.302103441</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>171</v>
+        <v>739</v>
       </c>
       <c r="B78" t="n">
-        <v>4.305664972</v>
+        <v>3.397338554</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>765</v>
+        <v>1213</v>
       </c>
       <c r="B79" t="n">
-        <v>5.507124664</v>
+        <v>7.907118123</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>919</v>
+        <v>393</v>
       </c>
       <c r="B80" t="n">
-        <v>3.515999317</v>
+        <v>4.252570445</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>125</v>
+        <v>664</v>
       </c>
       <c r="B81" t="n">
-        <v>5.608532732</v>
+        <v>22.2533743</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>1873</v>
+        <v>879</v>
       </c>
       <c r="B82" t="n">
-        <v>1.90688641</v>
+        <v>1.304019899</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>110</v>
+        <v>1232</v>
       </c>
       <c r="B83" t="n">
-        <v>4.119795432</v>
+        <v>1.643649533</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>832</v>
+        <v>1198</v>
       </c>
       <c r="B84" t="n">
-        <v>14.64996194</v>
+        <v>2.267031259</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>1157</v>
+        <v>814</v>
       </c>
       <c r="B85" t="n">
-        <v>4.128289298</v>
+        <v>2.392388585</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>1022</v>
+        <v>731</v>
       </c>
       <c r="B86" t="n">
-        <v>4.4150538</v>
+        <v>11.50518487</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>564</v>
+        <v>2</v>
       </c>
       <c r="B87" t="n">
-        <v>11.29322897</v>
+        <v>10.24419781</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>1298</v>
+        <v>16</v>
       </c>
       <c r="B88" t="n">
-        <v>2.040259928</v>
+        <v>1.524684145</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>379</v>
+        <v>1217</v>
       </c>
       <c r="B89" t="n">
-        <v>9.911599206</v>
+        <v>8.551846208000001</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>265</v>
+        <v>510</v>
       </c>
       <c r="B90" t="n">
-        <v>1.682853658</v>
+        <v>3.382248383</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>298</v>
+        <v>998</v>
       </c>
       <c r="B91" t="n">
-        <v>5.868904837</v>
+        <v>3.516954648</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>678</v>
+        <v>532</v>
       </c>
       <c r="B92" t="n">
-        <v>10.19830367</v>
+        <v>8.207253992</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>831</v>
+        <v>1257</v>
       </c>
       <c r="B93" t="n">
-        <v>19.03283303</v>
+        <v>10.93955763</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>604</v>
+        <v>268</v>
       </c>
       <c r="B94" t="n">
-        <v>18.44853818</v>
+        <v>3.800565648</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>182</v>
+        <v>495</v>
       </c>
       <c r="B95" t="n">
-        <v>7.085434186</v>
+        <v>9.134167683999999</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>590</v>
+        <v>1176</v>
       </c>
       <c r="B96" t="n">
-        <v>7.722099176</v>
+        <v>4.547074341</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>1281</v>
+        <v>796</v>
       </c>
       <c r="B97" t="n">
-        <v>13.51297643</v>
+        <v>16.78183408</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>325</v>
+        <v>937</v>
       </c>
       <c r="B98" t="n">
-        <v>5.728590451</v>
+        <v>15.16195083</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>694</v>
+        <v>1133</v>
       </c>
       <c r="B99" t="n">
-        <v>4.000152817</v>
+        <v>21.64834104</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>1315</v>
+        <v>969</v>
       </c>
       <c r="B100" t="n">
-        <v>7.426508774</v>
+        <v>16.16635264</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>1208</v>
+        <v>1260</v>
       </c>
       <c r="B101" t="n">
-        <v>3.919425327</v>
+        <v>4.354090239</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>21</v>
+        <v>520</v>
       </c>
       <c r="B102" t="n">
-        <v>1.968235026</v>
+        <v>5.88620926</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>1110</v>
+        <v>445</v>
       </c>
       <c r="B103" t="n">
-        <v>1.420416473</v>
+        <v>5.501719397</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>893</v>
+        <v>428</v>
       </c>
       <c r="B104" t="n">
-        <v>3.451730026</v>
+        <v>11.35448293</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>1135</v>
+        <v>692</v>
       </c>
       <c r="B105" t="n">
-        <v>7.630535538</v>
+        <v>2.602327942</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>1023</v>
+        <v>852</v>
       </c>
       <c r="B106" t="n">
-        <v>6.306234527</v>
+        <v>5.046586007</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>706</v>
+        <v>1283</v>
       </c>
       <c r="B107" t="n">
-        <v>6.298844699</v>
+        <v>24.64038811</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>801</v>
+        <v>1264</v>
       </c>
       <c r="B108" t="n">
-        <v>45.27448421</v>
+        <v>6.732542594</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>655</v>
+        <v>404</v>
       </c>
       <c r="B109" t="n">
-        <v>0.780461477</v>
+        <v>7.304546843</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>1148</v>
+        <v>873</v>
       </c>
       <c r="B110" t="n">
-        <v>8.265038085</v>
+        <v>8.776111974999999</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>393</v>
+        <v>1242</v>
       </c>
       <c r="B111" t="n">
-        <v>4.252570445</v>
+        <v>9.316208521</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>1235</v>
+        <v>231</v>
       </c>
       <c r="B112" t="n">
-        <v>19.25597407</v>
+        <v>3.193108236</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>1150</v>
+        <v>940</v>
       </c>
       <c r="B113" t="n">
-        <v>5.244472846</v>
+        <v>11.4919862</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>1202</v>
+        <v>383</v>
       </c>
       <c r="B114" t="n">
-        <v>6.572059975</v>
+        <v>26.66475114</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>222</v>
+        <v>451</v>
       </c>
       <c r="B115" t="n">
-        <v>14.41066927</v>
+        <v>4.293383604</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>998</v>
+        <v>1215</v>
       </c>
       <c r="B116" t="n">
-        <v>3.516954648</v>
+        <v>2.430772618</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>1053</v>
+        <v>552</v>
       </c>
       <c r="B117" t="n">
-        <v>0.607173883</v>
+        <v>25.53613408</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>1241</v>
+        <v>319</v>
       </c>
       <c r="B118" t="n">
-        <v>4.317230611</v>
+        <v>2.245353382</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>58</v>
+        <v>1098</v>
       </c>
       <c r="B119" t="n">
-        <v>3.704182734</v>
+        <v>16.92956402</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>1080</v>
+        <v>1159</v>
       </c>
       <c r="B120" t="n">
-        <v>10.44133384</v>
+        <v>26.54449129</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>504</v>
+        <v>1258</v>
       </c>
       <c r="B121" t="n">
-        <v>14.25321389</v>
+        <v>7.084729258</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>984</v>
+        <v>223</v>
       </c>
       <c r="B122" t="n">
-        <v>7.524731836</v>
+        <v>39.2450911</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>551</v>
+        <v>1003</v>
       </c>
       <c r="B123" t="n">
-        <v>7.936765267</v>
+        <v>1.026811435</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>0</v>
+        <v>580</v>
       </c>
       <c r="B124" t="n">
-        <v>8.422064636</v>
+        <v>7.337946605</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>549</v>
+        <v>1062</v>
       </c>
       <c r="B125" t="n">
-        <v>6.585174826</v>
+        <v>0.218340419</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>796</v>
+        <v>61</v>
       </c>
       <c r="B126" t="n">
-        <v>16.78183408</v>
+        <v>0.27875</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>331</v>
+        <v>502</v>
       </c>
       <c r="B127" t="n">
-        <v>4.556249266</v>
+        <v>11.8236877</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>1170</v>
+        <v>1244</v>
       </c>
       <c r="B128" t="n">
-        <v>11.35464727</v>
+        <v>11.94438288</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>56</v>
+        <v>1245</v>
       </c>
       <c r="B129" t="n">
-        <v>9.299167942</v>
+        <v>17.12941674</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>1217</v>
+        <v>349</v>
       </c>
       <c r="B130" t="n">
-        <v>8.551846208000001</v>
+        <v>20.70055083</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>1265</v>
+        <v>1136</v>
       </c>
       <c r="B131" t="n">
-        <v>14.84067376</v>
+        <v>5.927035504</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>92</v>
+        <v>1856</v>
       </c>
       <c r="B132" t="n">
-        <v>9.361645508000001</v>
+        <v>6.783337842</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>1206</v>
+        <v>549</v>
       </c>
       <c r="B133" t="n">
-        <v>2.875195382</v>
+        <v>6.585174826</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>663</v>
+        <v>589</v>
       </c>
       <c r="B134" t="n">
-        <v>13.81309878</v>
+        <v>11.38852803</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>649</v>
+        <v>573</v>
       </c>
       <c r="B135" t="n">
-        <v>3.592411721</v>
+        <v>6.425386489</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>39</v>
+        <v>1010</v>
       </c>
       <c r="B136" t="n">
-        <v>5.767574894</v>
+        <v>16.68671935</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>863</v>
+        <v>1137</v>
       </c>
       <c r="B137" t="n">
-        <v>6.312758056</v>
+        <v>3.938286344</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>1515</v>
+        <v>340</v>
       </c>
       <c r="B138" t="n">
-        <v>1.241706504</v>
+        <v>1.760727191</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>1294</v>
+        <v>246</v>
       </c>
       <c r="B139" t="n">
-        <v>4.715966204</v>
+        <v>5.954562531</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>548</v>
+        <v>147</v>
       </c>
       <c r="B140" t="n">
-        <v>5.893807862</v>
+        <v>27.75018732</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>422</v>
+        <v>1299</v>
       </c>
       <c r="B141" t="n">
-        <v>19.60390138</v>
+        <v>4.410310579</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>1195</v>
+        <v>1112</v>
       </c>
       <c r="B142" t="n">
-        <v>1.791163332</v>
+        <v>3.583791072</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>292</v>
+        <v>681</v>
       </c>
       <c r="B143" t="n">
-        <v>3.516943532</v>
+        <v>4.174533061</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>1508</v>
+        <v>1868</v>
       </c>
       <c r="B144" t="n">
-        <v>5.593399546</v>
+        <v>15.53263525</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>199</v>
+        <v>67</v>
       </c>
       <c r="B145" t="n">
-        <v>6.176411989</v>
+        <v>8.756613014999999</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>1874</v>
+        <v>111</v>
       </c>
       <c r="B146" t="n">
-        <v>2.254280661</v>
+        <v>8.251959846</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>485</v>
+        <v>1562</v>
       </c>
       <c r="B147" t="n">
-        <v>5.355498109</v>
+        <v>5.674373444</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>1027</v>
+        <v>515</v>
       </c>
       <c r="B148" t="n">
-        <v>3.48814515</v>
+        <v>6.939758772</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>1310</v>
+        <v>1023</v>
       </c>
       <c r="B149" t="n">
-        <v>8.575790831999999</v>
+        <v>6.306234527</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>146</v>
+        <v>829</v>
       </c>
       <c r="B150" t="n">
-        <v>56.08509159</v>
+        <v>12.7521176</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>1312</v>
+        <v>210</v>
       </c>
       <c r="B151" t="n">
-        <v>15.50679647</v>
+        <v>2.370623479</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>357</v>
+        <v>1504</v>
       </c>
       <c r="B152" t="n">
-        <v>5.718274897</v>
+        <v>5.847473201</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>1233</v>
+        <v>1285</v>
       </c>
       <c r="B153" t="n">
-        <v>8.50162531</v>
+        <v>6.086451365</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>1558</v>
+        <v>870</v>
       </c>
       <c r="B154" t="n">
-        <v>6.923547824</v>
+        <v>4.513937665</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>163</v>
+        <v>1878</v>
       </c>
       <c r="B155" t="n">
-        <v>5.747322623</v>
+        <v>4.544644752</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>994</v>
+        <v>443</v>
       </c>
       <c r="B156" t="n">
-        <v>2.206427225</v>
+        <v>1.735039599</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>1074</v>
+        <v>1224</v>
       </c>
       <c r="B157" t="n">
-        <v>10.59243092</v>
+        <v>3.187508609</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>1121</v>
+        <v>574</v>
       </c>
       <c r="B158" t="n">
-        <v>7.753343084</v>
+        <v>11.27096667</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>961</v>
+        <v>1122</v>
       </c>
       <c r="B159" t="n">
-        <v>9.541877105999999</v>
+        <v>7.266623176</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>1514</v>
+        <v>92</v>
       </c>
       <c r="B160" t="n">
-        <v>2.923991011</v>
+        <v>9.361645508000001</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>995</v>
+        <v>171</v>
       </c>
       <c r="B161" t="n">
-        <v>3.933971262</v>
+        <v>4.305664972</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>244</v>
+        <v>1252</v>
       </c>
       <c r="B162" t="n">
-        <v>8.333593296</v>
+        <v>24.50463812</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>1221</v>
+        <v>255</v>
       </c>
       <c r="B163" t="n">
-        <v>18.16059629</v>
+        <v>5.869996102</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>651</v>
+        <v>1100</v>
       </c>
       <c r="B164" t="n">
-        <v>1.542364563</v>
+        <v>7.582783708</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>1087</v>
+        <v>1888</v>
       </c>
       <c r="B165" t="n">
-        <v>19.30242725</v>
+        <v>8.259115013000001</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>81</v>
+        <v>1030</v>
       </c>
       <c r="B166" t="n">
-        <v>7.002961284</v>
+        <v>5.628969187</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="B167" t="n">
-        <v>10.77448021</v>
+        <v>3.960859807</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>517</v>
+        <v>427</v>
       </c>
       <c r="B168" t="n">
-        <v>15.68333812</v>
+        <v>4.178800085</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
-        <v>79</v>
+        <v>1080</v>
       </c>
       <c r="B169" t="n">
-        <v>6.213209469</v>
+        <v>10.44133384</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
-        <v>937</v>
+        <v>126</v>
       </c>
       <c r="B170" t="n">
-        <v>15.16195083</v>
+        <v>13.1422193</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>722</v>
+        <v>1148</v>
       </c>
       <c r="B171" t="n">
-        <v>5.255192675</v>
+        <v>8.265038085</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>664</v>
+        <v>560</v>
       </c>
       <c r="B172" t="n">
-        <v>22.2533743</v>
+        <v>5.992360715</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>965</v>
+        <v>131</v>
       </c>
       <c r="B173" t="n">
-        <v>8.051653369</v>
+        <v>16.65504216</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>202</v>
+        <v>657</v>
       </c>
       <c r="B174" t="n">
-        <v>15.35336526</v>
+        <v>8.202778093999999</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
-        <v>418</v>
+        <v>365</v>
       </c>
       <c r="B175" t="n">
-        <v>9.871273872</v>
+        <v>7.548358182</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>3</v>
+        <v>1082</v>
       </c>
       <c r="B176" t="n">
-        <v>7.893081934</v>
+        <v>2.325112666</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>12</v>
+        <v>256</v>
       </c>
       <c r="B177" t="n">
-        <v>6.628267212</v>
+        <v>11.70031429</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
-        <v>1154</v>
+        <v>938</v>
       </c>
       <c r="B178" t="n">
-        <v>3.00723487</v>
+        <v>10.76676513</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>305</v>
+        <v>825</v>
       </c>
       <c r="B179" t="n">
-        <v>11.34589481</v>
+        <v>8.943062529000001</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>764</v>
+        <v>983</v>
       </c>
       <c r="B180" t="n">
-        <v>9.197091886999999</v>
+        <v>6.168505989</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>516</v>
+        <v>1270</v>
       </c>
       <c r="B181" t="n">
-        <v>11.96201208</v>
+        <v>23.77493671</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>892</v>
+        <v>1908</v>
       </c>
       <c r="B182" t="n">
-        <v>3.379699033</v>
+        <v>3.291428304</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>1856</v>
+        <v>158</v>
       </c>
       <c r="B183" t="n">
-        <v>6.783337842</v>
+        <v>34.65335182</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
-        <v>784</v>
+        <v>1044</v>
       </c>
       <c r="B184" t="n">
-        <v>3.154616194</v>
+        <v>12.05217344</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>1075</v>
+        <v>28</v>
       </c>
       <c r="B185" t="n">
-        <v>11.22339524</v>
+        <v>2.772930116</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
-        <v>834</v>
+        <v>444</v>
       </c>
       <c r="B186" t="n">
-        <v>10.1797811</v>
+        <v>3.606418592</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
-        <v>1864</v>
+        <v>1879</v>
       </c>
       <c r="B187" t="n">
-        <v>6.938495397</v>
+        <v>3.3196347</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>1545</v>
+        <v>916</v>
       </c>
       <c r="B188" t="n">
-        <v>5.094255712</v>
+        <v>1.879472035</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>468</v>
+        <v>1915</v>
       </c>
       <c r="B189" t="n">
-        <v>9.204340435000001</v>
+        <v>9.67293761</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>1236</v>
+        <v>521</v>
       </c>
       <c r="B190" t="n">
-        <v>7.262603517</v>
+        <v>7.384093361</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>212</v>
+        <v>1313</v>
       </c>
       <c r="B191" t="n">
-        <v>4.149723633</v>
+        <v>7.866193029</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
-        <v>1904</v>
+        <v>910</v>
       </c>
       <c r="B192" t="n">
-        <v>7.794791907</v>
+        <v>9.123956811999999</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>1167</v>
+        <v>1125</v>
       </c>
       <c r="B193" t="n">
-        <v>21.24727776</v>
+        <v>4.452775966</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>1094</v>
+        <v>618</v>
       </c>
       <c r="B194" t="n">
-        <v>9.457559951</v>
+        <v>3.946696433</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
-        <v>482</v>
+        <v>80</v>
       </c>
       <c r="B195" t="n">
-        <v>66.20402687000001</v>
+        <v>9.373180065</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
-        <v>554</v>
+        <v>1013</v>
       </c>
       <c r="B196" t="n">
-        <v>4.400345325</v>
+        <v>7.107049538</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
-        <v>1550</v>
+        <v>774</v>
       </c>
       <c r="B197" t="n">
-        <v>6.577247291</v>
+        <v>1.396188362</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
-        <v>344</v>
+        <v>137</v>
       </c>
       <c r="B198" t="n">
-        <v>16.97827624</v>
+        <v>9.589548835</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
-        <v>1905</v>
+        <v>1014</v>
       </c>
       <c r="B199" t="n">
-        <v>4.246744498</v>
+        <v>8.225421277000001</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
-        <v>508</v>
+        <v>264</v>
       </c>
       <c r="B200" t="n">
-        <v>5.917760572</v>
+        <v>5.686513047</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
-        <v>874</v>
+        <v>978</v>
       </c>
       <c r="B201" t="n">
-        <v>3.398649395</v>
+        <v>5.098237971</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>620</v>
+        <v>847</v>
       </c>
       <c r="B202" t="n">
-        <v>12.67827277</v>
+        <v>3.636419977</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>1561</v>
+        <v>439</v>
       </c>
       <c r="B203" t="n">
-        <v>7.446748488</v>
+        <v>2.939331368</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>239</v>
+        <v>984</v>
       </c>
       <c r="B204" t="n">
-        <v>2.299742102</v>
+        <v>7.524731836</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>1123</v>
+        <v>1093</v>
       </c>
       <c r="B205" t="n">
-        <v>3.506780718</v>
+        <v>18.94784243</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>63</v>
+        <v>890</v>
       </c>
       <c r="B206" t="n">
-        <v>12.36270136</v>
+        <v>2.197175703</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>929</v>
+        <v>25</v>
       </c>
       <c r="B207" t="n">
-        <v>2.348164872</v>
+        <v>15.64952857</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>1112</v>
+        <v>1103</v>
       </c>
       <c r="B208" t="n">
-        <v>3.583791072</v>
+        <v>4.080288815</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>141</v>
+        <v>1153</v>
       </c>
       <c r="B209" t="n">
-        <v>4.486268468</v>
+        <v>2.762870125</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>210</v>
+        <v>1042</v>
       </c>
       <c r="B210" t="n">
-        <v>2.370623479</v>
+        <v>7.033167023</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>269</v>
+        <v>799</v>
       </c>
       <c r="B211" t="n">
-        <v>11.00657433</v>
+        <v>13.11734684</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>102</v>
+        <v>1162</v>
       </c>
       <c r="B212" t="n">
-        <v>6.651263691</v>
+        <v>13.45629827</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>1038</v>
+        <v>1294</v>
       </c>
       <c r="B213" t="n">
-        <v>4.282608197</v>
+        <v>4.715966204</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>1026</v>
+        <v>700</v>
       </c>
       <c r="B214" t="n">
-        <v>4.823260956</v>
+        <v>1.059760245</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>922</v>
+        <v>382</v>
       </c>
       <c r="B215" t="n">
-        <v>7.588971112</v>
+        <v>11.84391172</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>436</v>
+        <v>585</v>
       </c>
       <c r="B216" t="n">
-        <v>15.75945716</v>
+        <v>2.084117348</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>1081</v>
+        <v>509</v>
       </c>
       <c r="B217" t="n">
-        <v>3.216697166</v>
+        <v>10.90215141</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>397</v>
+        <v>1256</v>
       </c>
       <c r="B218" t="n">
-        <v>5.860503031</v>
+        <v>3.799273955</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
-        <v>200</v>
+        <v>652</v>
       </c>
       <c r="B219" t="n">
-        <v>6.363634576</v>
+        <v>4.044214675</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>875</v>
+        <v>238</v>
       </c>
       <c r="B220" t="n">
-        <v>3.191287868</v>
+        <v>3.280633393</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>243</v>
+        <v>1276</v>
       </c>
       <c r="B221" t="n">
-        <v>7.37537074</v>
+        <v>5.302086094</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>1103</v>
+        <v>715</v>
       </c>
       <c r="B222" t="n">
-        <v>4.080288815</v>
+        <v>6.457262046</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>1109</v>
+        <v>981</v>
       </c>
       <c r="B223" t="n">
-        <v>5.265473643</v>
+        <v>3.266672805</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>1230</v>
+        <v>1038</v>
       </c>
       <c r="B224" t="n">
-        <v>13.43379293</v>
+        <v>4.282608197</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>703</v>
+        <v>887</v>
       </c>
       <c r="B225" t="n">
-        <v>2.4483074</v>
+        <v>5.282127523</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>178</v>
+        <v>1076</v>
       </c>
       <c r="B226" t="n">
-        <v>8.775490261</v>
+        <v>13.74684936</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>415</v>
+        <v>437</v>
       </c>
       <c r="B227" t="n">
-        <v>3.723703389</v>
+        <v>22.28714236</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>1205</v>
+        <v>839</v>
       </c>
       <c r="B228" t="n">
-        <v>4.942861368</v>
+        <v>8.799365691</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>183</v>
+        <v>1128</v>
       </c>
       <c r="B229" t="n">
-        <v>7.57637515</v>
+        <v>7.320554146</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>1512</v>
+        <v>213</v>
       </c>
       <c r="B230" t="n">
-        <v>3.225325189</v>
+        <v>3.378061513</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>518</v>
+        <v>745</v>
       </c>
       <c r="B231" t="n">
-        <v>10.97908896</v>
+        <v>3.366535124</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>589</v>
+        <v>767</v>
       </c>
       <c r="B232" t="n">
-        <v>11.38852803</v>
+        <v>2.031511318</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>524</v>
+        <v>701</v>
       </c>
       <c r="B233" t="n">
-        <v>1.552124508</v>
+        <v>1.377728144</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>1024</v>
+        <v>988</v>
       </c>
       <c r="B234" t="n">
-        <v>10.03780942</v>
+        <v>11.76704502</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>1253</v>
+        <v>183</v>
       </c>
       <c r="B235" t="n">
-        <v>7.018089904</v>
+        <v>7.57637515</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>324</v>
+        <v>224</v>
       </c>
       <c r="B236" t="n">
-        <v>5.072832642</v>
+        <v>18.57519341</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>630</v>
+        <v>1204</v>
       </c>
       <c r="B237" t="n">
-        <v>10.5803892</v>
+        <v>34.73312758</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>1256</v>
+        <v>1898</v>
       </c>
       <c r="B238" t="n">
-        <v>3.799273955</v>
+        <v>2.43695945</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>529</v>
+        <v>280</v>
       </c>
       <c r="B239" t="n">
-        <v>1.983768609</v>
+        <v>7.368192608</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>313</v>
+        <v>1311</v>
       </c>
       <c r="B240" t="n">
-        <v>6.623461771</v>
+        <v>8.258760962</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>1131</v>
+        <v>1220</v>
       </c>
       <c r="B241" t="n">
-        <v>12.68248508</v>
+        <v>12.37984207</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>1270</v>
+        <v>666</v>
       </c>
       <c r="B242" t="n">
-        <v>23.77493671</v>
+        <v>7.528913847</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>1047</v>
+        <v>607</v>
       </c>
       <c r="B243" t="n">
-        <v>0.921319068</v>
+        <v>7.198093831</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>536</v>
+        <v>1247</v>
       </c>
       <c r="B244" t="n">
-        <v>9.919362102999999</v>
+        <v>12.20270761</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>1043</v>
+        <v>1858</v>
       </c>
       <c r="B245" t="n">
-        <v>7.001765162</v>
+        <v>10.26421971</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>1212</v>
+        <v>601</v>
       </c>
       <c r="B246" t="n">
-        <v>6.92781315</v>
+        <v>1.762187374</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="B247" t="n">
-        <v>21.20265521</v>
+        <v>3.83184061</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>266</v>
+        <v>850</v>
       </c>
       <c r="B248" t="n">
-        <v>0.116309274</v>
+        <v>5.85783368</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>382</v>
+        <v>533</v>
       </c>
       <c r="B249" t="n">
-        <v>11.84391172</v>
+        <v>11.45365705</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="B250" t="n">
-        <v>6.380772234</v>
+        <v>13.00399896</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>772</v>
+        <v>971</v>
       </c>
       <c r="B251" t="n">
-        <v>1.236380128</v>
+        <v>2.150049135</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>653</v>
+        <v>943</v>
       </c>
       <c r="B252" t="n">
-        <v>4.149255304</v>
+        <v>35.96689981</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>78</v>
+        <v>450</v>
       </c>
       <c r="B253" t="n">
-        <v>3.869189366</v>
+        <v>5.073046797</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B254" t="n">
-        <v>6.137564282</v>
+        <v>11.34589481</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>1901</v>
+        <v>865</v>
       </c>
       <c r="B255" t="n">
-        <v>2.443573166</v>
+        <v>8.014607505000001</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
-        <v>734</v>
+        <v>563</v>
       </c>
       <c r="B256" t="n">
-        <v>20.83637147</v>
+        <v>31.50094811</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
-        <v>1895</v>
+        <v>1489</v>
       </c>
       <c r="B257" t="n">
-        <v>2.214552252</v>
+        <v>11.37181113</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>741</v>
+        <v>874</v>
       </c>
       <c r="B258" t="n">
-        <v>7.04373661</v>
+        <v>3.398649395</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>845</v>
+        <v>1063</v>
       </c>
       <c r="B259" t="n">
-        <v>3.77125118</v>
+        <v>7.347076112</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>618</v>
+        <v>265</v>
       </c>
       <c r="B260" t="n">
-        <v>3.946696433</v>
+        <v>1.682853658</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>149</v>
+        <v>1873</v>
       </c>
       <c r="B261" t="n">
-        <v>3.286599325</v>
+        <v>1.90688641</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>767</v>
+        <v>1527</v>
       </c>
       <c r="B262" t="n">
-        <v>2.031511318</v>
+        <v>0.717175871</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>594</v>
+        <v>1513</v>
       </c>
       <c r="B263" t="n">
-        <v>10.32004246</v>
+        <v>1.373628596</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>843</v>
+        <v>514</v>
       </c>
       <c r="B264" t="n">
-        <v>4.719541631</v>
+        <v>4.206054306</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>1870</v>
+        <v>842</v>
       </c>
       <c r="B265" t="n">
-        <v>9.076710616</v>
+        <v>0.918832627</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>1119</v>
+        <v>1073</v>
       </c>
       <c r="B266" t="n">
-        <v>8.436594728999999</v>
+        <v>6.872368933</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="B267" t="n">
-        <v>12.37242061</v>
+        <v>5.670344795</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>755</v>
+        <v>1882</v>
       </c>
       <c r="B268" t="n">
-        <v>16.58343578</v>
+        <v>11.35195954</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>369</v>
+        <v>1114</v>
       </c>
       <c r="B269" t="n">
-        <v>3.215905681</v>
+        <v>8.373434768999999</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>22</v>
+        <v>1143</v>
       </c>
       <c r="B270" t="n">
-        <v>1.689171042</v>
+        <v>2.185066883</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>915</v>
+        <v>143</v>
       </c>
       <c r="B271" t="n">
-        <v>6.713584882</v>
+        <v>7.448219881</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>147</v>
+        <v>726</v>
       </c>
       <c r="B272" t="n">
-        <v>27.75018732</v>
+        <v>3.797313285</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>1886</v>
+        <v>1310</v>
       </c>
       <c r="B273" t="n">
-        <v>5.49698452</v>
+        <v>8.575790831999999</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
-        <v>882</v>
+        <v>201</v>
       </c>
       <c r="B274" t="n">
-        <v>0.85139524</v>
+        <v>7.10658818</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
-        <v>499</v>
+        <v>1284</v>
       </c>
       <c r="B275" t="n">
-        <v>1.78924921</v>
+        <v>5.496510121</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
-        <v>753</v>
+        <v>991</v>
       </c>
       <c r="B276" t="n">
-        <v>13.20509137</v>
+        <v>9.152991543000001</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>152</v>
+        <v>1177</v>
       </c>
       <c r="B277" t="n">
-        <v>3.448185178</v>
+        <v>12.40086561</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
-        <v>375</v>
+        <v>422</v>
       </c>
       <c r="B278" t="n">
-        <v>15.5677777</v>
+        <v>19.60390138</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
-        <v>546</v>
+        <v>703</v>
       </c>
       <c r="B279" t="n">
-        <v>4.169698838</v>
+        <v>2.4483074</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
-        <v>657</v>
+        <v>1006</v>
       </c>
       <c r="B280" t="n">
-        <v>8.202778093999999</v>
+        <v>0.240036866</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
-        <v>829</v>
+        <v>1237</v>
       </c>
       <c r="B281" t="n">
-        <v>12.7521176</v>
+        <v>3.537484358</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>437</v>
+        <v>565</v>
       </c>
       <c r="B282" t="n">
-        <v>22.28714236</v>
+        <v>13.23858641</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>522</v>
+        <v>859</v>
       </c>
       <c r="B283" t="n">
-        <v>3.2624933</v>
+        <v>2.237461923</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
-        <v>885</v>
+        <v>1155</v>
       </c>
       <c r="B284" t="n">
-        <v>8.132012255999999</v>
+        <v>0.885496578</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
-        <v>73</v>
+        <v>734</v>
       </c>
       <c r="B285" t="n">
-        <v>1.045292237</v>
+        <v>20.83637147</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
-        <v>33</v>
+        <v>316</v>
       </c>
       <c r="B286" t="n">
-        <v>12.57367205</v>
+        <v>4.25599037</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
-        <v>941</v>
+        <v>10</v>
       </c>
       <c r="B287" t="n">
-        <v>6.918548492</v>
+        <v>9.867879654999999</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
-        <v>987</v>
+        <v>1205</v>
       </c>
       <c r="B288" t="n">
-        <v>16.65102368</v>
+        <v>4.942861368</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
-        <v>1898</v>
+        <v>114</v>
       </c>
       <c r="B289" t="n">
-        <v>2.43695945</v>
+        <v>4.79399121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>